<commit_message>
Fix: Checks if the person is on the do not handle list. If the person is present, it is not sent up the queue.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Carl\Lärarkostnad per gymnasieprogram\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\Theresia\RPA-LararKostnadPerGymnasieprogram-Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>ProgramKoder_FilePath</t>
+  </si>
+  <si>
+    <t>Cred_APIGateway_Prod</t>
+  </si>
+  <si>
+    <t>FilePathToBlackList</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -630,7 +636,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2797,7 +2810,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2860,7 +2873,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>